<commit_message>
add test for generating order spreadsheet
</commit_message>
<xml_diff>
--- a/packages/lambda-kit-orders-create/ORDER FORM.xlsx
+++ b/packages/lambda-kit-orders-create/ORDER FORM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="586">
   <si>
     <t>Code</t>
   </si>
@@ -509,6 +509,24 @@
     <t xml:space="preserve">Skinsuit S/S ELITE-A 38 | Lycra POWER </t>
   </si>
   <si>
+    <t>n56018-MA02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit S/S ELITE-A 02 | Lycra POWER </t>
+  </si>
+  <si>
+    <t>Endurance 3D pad, one small back pocket</t>
+  </si>
+  <si>
+    <t>n56018-MA37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit S/S ELITE-A 37 | Lycra POWER </t>
+  </si>
+  <si>
+    <t>Zoom X pad, one small back pocket</t>
+  </si>
+  <si>
     <t>n56028-MA03</t>
   </si>
   <si>
@@ -521,6 +539,18 @@
     <t xml:space="preserve">Skinsuit L/S ELITE-A 38 | Lycra POWER </t>
   </si>
   <si>
+    <t>n56028-MA02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit L/S ELITE-A 02 | Lycra POWER </t>
+  </si>
+  <si>
+    <t>n56028-MA37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit L/S ELITE-A 37 | Lycra POWER </t>
+  </si>
+  <si>
     <t>n56016-MA03</t>
   </si>
   <si>
@@ -533,6 +563,18 @@
     <t xml:space="preserve">Skinsuit S/S ELITE-A 38 | REVOLUTIONAL </t>
   </si>
   <si>
+    <t>n56016-MA02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit S/S ELITE-A 02 | REVOLUTIONAL </t>
+  </si>
+  <si>
+    <t>n56016-MA37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit S/S ELITE-A 37 | REVOLUTIONAL </t>
+  </si>
+  <si>
     <t>n56026-MA03</t>
   </si>
   <si>
@@ -548,6 +590,18 @@
     <t>Zoom x pad</t>
   </si>
   <si>
+    <t>n56026-MA02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit L/S ELITE-A 02 | REVOLUTIONAL </t>
+  </si>
+  <si>
+    <t>n56026-MA37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit L/S ELITE-A 37 | REVOLUTIONAL </t>
+  </si>
+  <si>
     <t>PRO COLLECTION</t>
   </si>
   <si>
@@ -1001,6 +1055,24 @@
     <t xml:space="preserve">Skinsuit S/S ELITE-A 34 | Lycra POWER </t>
   </si>
   <si>
+    <t>n56018-UA33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit S/S ELITE-A 33 | Lycra POWER </t>
+  </si>
+  <si>
+    <t>Endurance 3D women pad, one small back pocket</t>
+  </si>
+  <si>
+    <t>n56018-UA32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit S/S ELITE-A 32 | Lycra POWER </t>
+  </si>
+  <si>
+    <t>Zoom X women pad, one small back pocket</t>
+  </si>
+  <si>
     <t>n56028-UA35</t>
   </si>
   <si>
@@ -1013,6 +1085,18 @@
     <t xml:space="preserve">Skinsuit L/S ELITE-A 34 | Lycra POWER </t>
   </si>
   <si>
+    <t>n56028-UA33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit L/S ELITE-A 33 | Lycra POWER </t>
+  </si>
+  <si>
+    <t>n56028-UA32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit L/S ELITE-A 32 | Lycra POWER </t>
+  </si>
+  <si>
     <t>n56016-UA35</t>
   </si>
   <si>
@@ -1025,6 +1109,18 @@
     <t xml:space="preserve">Skinsuit S/S ELITE-A 34 | REVOLUTIONAL </t>
   </si>
   <si>
+    <t>n56016-UA33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit S/S ELITE-A 33 | REVOLUTIONAL </t>
+  </si>
+  <si>
+    <t>n56016-UA32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit S/S ELITE-A 32 | REVOLUTIONAL </t>
+  </si>
+  <si>
     <t>n56026-UA35</t>
   </si>
   <si>
@@ -1035,6 +1131,18 @@
   </si>
   <si>
     <t xml:space="preserve">Skinsuit L/S ELITE-A 34 | REVOLUTIONAL </t>
+  </si>
+  <si>
+    <t>n56026-UA33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit L/S ELITE-A 33 | REVOLUTIONAL </t>
+  </si>
+  <si>
+    <t>n56026-UA32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinsuit L/S ELITE-A 32 | REVOLUTIONAL </t>
   </si>
   <si>
     <t>n56069-JA27</t>
@@ -3338,7 +3446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -5314,7 +5422,7 @@
         <v>165</v>
       </c>
       <c r="C73" t="s" s="19">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="D73" s="17"/>
       <c r="E73" s="17"/>
@@ -5335,13 +5443,13 @@
     </row>
     <row r="74" ht="16" customHeight="1">
       <c r="A74" t="s" s="19">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s" s="20">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C74" t="s" s="19">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
@@ -5362,10 +5470,10 @@
     </row>
     <row r="75" ht="16" customHeight="1">
       <c r="A75" t="s" s="19">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B75" t="s" s="20">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C75" t="s" s="19">
         <v>45</v>
@@ -5389,10 +5497,10 @@
     </row>
     <row r="76" ht="16" customHeight="1">
       <c r="A76" t="s" s="19">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B76" t="s" s="20">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C76" t="s" s="19">
         <v>48</v>
@@ -5416,13 +5524,13 @@
     </row>
     <row r="77" ht="16" customHeight="1">
       <c r="A77" t="s" s="19">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B77" t="s" s="20">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C77" t="s" s="19">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
@@ -5443,13 +5551,13 @@
     </row>
     <row r="78" ht="16" customHeight="1">
       <c r="A78" t="s" s="19">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B78" t="s" s="20">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C78" t="s" s="19">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D78" s="17"/>
       <c r="E78" s="17"/>
@@ -5469,58 +5577,274 @@
       </c>
     </row>
     <row r="79" ht="16" customHeight="1">
-      <c r="A79" s="21"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="21"/>
+      <c r="A79" t="s" s="19">
+        <v>178</v>
+      </c>
+      <c r="B79" t="s" s="20">
+        <v>179</v>
+      </c>
+      <c r="C79" t="s" s="19">
+        <v>45</v>
+      </c>
       <c r="D79" s="17"/>
       <c r="E79" s="17"/>
       <c r="F79" s="17"/>
       <c r="G79" s="17"/>
       <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="17"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="25"/>
+      <c r="K79" s="25"/>
+      <c r="L79" s="26"/>
       <c r="M79" s="17"/>
       <c r="N79" s="17"/>
       <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
+      <c r="P79" s="18">
+        <f>SUM(D79:O79)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="80" ht="16" customHeight="1">
-      <c r="A80" s="21"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="21"/>
+      <c r="A80" t="s" s="19">
+        <v>180</v>
+      </c>
+      <c r="B80" t="s" s="20">
+        <v>181</v>
+      </c>
+      <c r="C80" t="s" s="19">
+        <v>48</v>
+      </c>
       <c r="D80" s="17"/>
       <c r="E80" s="17"/>
       <c r="F80" s="17"/>
       <c r="G80" s="17"/>
       <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="17"/>
-      <c r="L80" s="17"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="25"/>
+      <c r="K80" s="25"/>
+      <c r="L80" s="26"/>
       <c r="M80" s="17"/>
       <c r="N80" s="17"/>
       <c r="O80" s="17"/>
-      <c r="P80" s="17"/>
+      <c r="P80" s="18">
+        <f>SUM(D80:O80)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="81" ht="16" customHeight="1">
-      <c r="A81" s="21"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
+      <c r="A81" t="s" s="19">
+        <v>182</v>
+      </c>
+      <c r="B81" t="s" s="20">
+        <v>183</v>
+      </c>
+      <c r="C81" t="s" s="19">
+        <v>166</v>
+      </c>
       <c r="D81" s="17"/>
       <c r="E81" s="17"/>
       <c r="F81" s="17"/>
       <c r="G81" s="17"/>
       <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="17"/>
-      <c r="L81" s="17"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="25"/>
+      <c r="K81" s="25"/>
+      <c r="L81" s="26"/>
       <c r="M81" s="17"/>
       <c r="N81" s="17"/>
       <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
+      <c r="P81" s="18">
+        <f>SUM(D81:O81)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" ht="16" customHeight="1">
+      <c r="A82" t="s" s="19">
+        <v>184</v>
+      </c>
+      <c r="B82" t="s" s="20">
+        <v>185</v>
+      </c>
+      <c r="C82" t="s" s="19">
+        <v>169</v>
+      </c>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="24"/>
+      <c r="J82" s="25"/>
+      <c r="K82" s="25"/>
+      <c r="L82" s="26"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="18">
+        <f>SUM(D82:O82)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" ht="16" customHeight="1">
+      <c r="A83" t="s" s="19">
+        <v>186</v>
+      </c>
+      <c r="B83" t="s" s="20">
+        <v>187</v>
+      </c>
+      <c r="C83" t="s" s="19">
+        <v>45</v>
+      </c>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="25"/>
+      <c r="K83" s="25"/>
+      <c r="L83" s="26"/>
+      <c r="M83" s="17"/>
+      <c r="N83" s="17"/>
+      <c r="O83" s="17"/>
+      <c r="P83" s="18">
+        <f>SUM(D83:O83)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" ht="16" customHeight="1">
+      <c r="A84" t="s" s="19">
+        <v>188</v>
+      </c>
+      <c r="B84" t="s" s="20">
+        <v>189</v>
+      </c>
+      <c r="C84" t="s" s="19">
+        <v>190</v>
+      </c>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="25"/>
+      <c r="K84" s="25"/>
+      <c r="L84" s="26"/>
+      <c r="M84" s="17"/>
+      <c r="N84" s="17"/>
+      <c r="O84" s="17"/>
+      <c r="P84" s="18">
+        <f>SUM(D84:O84)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" ht="16" customHeight="1">
+      <c r="A85" t="s" s="19">
+        <v>191</v>
+      </c>
+      <c r="B85" t="s" s="20">
+        <v>192</v>
+      </c>
+      <c r="C85" t="s" s="19">
+        <v>166</v>
+      </c>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="25"/>
+      <c r="K85" s="25"/>
+      <c r="L85" s="26"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="18">
+        <f>SUM(D85:O85)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" ht="16" customHeight="1">
+      <c r="A86" t="s" s="19">
+        <v>193</v>
+      </c>
+      <c r="B86" t="s" s="20">
+        <v>194</v>
+      </c>
+      <c r="C86" t="s" s="19">
+        <v>169</v>
+      </c>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="25"/>
+      <c r="K86" s="25"/>
+      <c r="L86" s="26"/>
+      <c r="M86" s="17"/>
+      <c r="N86" s="17"/>
+      <c r="O86" s="17"/>
+      <c r="P86" s="18">
+        <f>SUM(D86:O86)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" ht="16" customHeight="1">
+      <c r="A87" s="21"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="17"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
+    </row>
+    <row r="88" ht="16" customHeight="1">
+      <c r="A88" s="21"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
+      <c r="J88" s="17"/>
+      <c r="K88" s="17"/>
+      <c r="L88" s="17"/>
+      <c r="M88" s="17"/>
+      <c r="N88" s="17"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="17"/>
+    </row>
+    <row r="89" ht="16" customHeight="1">
+      <c r="A89" s="21"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
+      <c r="J89" s="17"/>
+      <c r="K89" s="17"/>
+      <c r="L89" s="17"/>
+      <c r="M89" s="17"/>
+      <c r="N89" s="17"/>
+      <c r="O89" s="17"/>
+      <c r="P89" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5536,7 +5860,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P99"/>
+  <dimension ref="A1:P107"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -5580,7 +5904,7 @@
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -5624,7 +5948,7 @@
     </row>
     <row r="3" ht="16" customHeight="1">
       <c r="A3" t="s" s="14">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s" s="15">
         <v>11</v>
@@ -5649,7 +5973,7 @@
     </row>
     <row r="4" ht="16" customHeight="1">
       <c r="A4" t="s" s="19">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s" s="20">
         <v>13</v>
@@ -5676,7 +6000,7 @@
     </row>
     <row r="5" ht="16" customHeight="1">
       <c r="A5" t="s" s="19">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s" s="20">
         <v>16</v>
@@ -5701,7 +6025,7 @@
     </row>
     <row r="6" ht="16" customHeight="1">
       <c r="A6" t="s" s="19">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s" s="20">
         <v>18</v>
@@ -5728,7 +6052,7 @@
     </row>
     <row r="7" ht="16" customHeight="1">
       <c r="A7" t="s" s="19">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s" s="20">
         <v>20</v>
@@ -5753,10 +6077,10 @@
     </row>
     <row r="8" ht="16" customHeight="1">
       <c r="A8" t="s" s="19">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="B8" t="s" s="20">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s" s="19">
         <v>14</v>
@@ -5780,10 +6104,10 @@
     </row>
     <row r="9" ht="16" customHeight="1">
       <c r="A9" t="s" s="19">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="B9" t="s" s="20">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="17"/>
@@ -5805,7 +6129,7 @@
     </row>
     <row r="10" ht="16" customHeight="1">
       <c r="A10" t="s" s="19">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="B10" t="s" s="20">
         <v>26</v>
@@ -5830,7 +6154,7 @@
     </row>
     <row r="11" ht="16" customHeight="1">
       <c r="A11" t="s" s="19">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="B11" t="s" s="20">
         <v>28</v>
@@ -5855,10 +6179,10 @@
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" t="s" s="19">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="B12" t="s" s="20">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="17"/>
@@ -5880,7 +6204,7 @@
     </row>
     <row r="13" ht="16" customHeight="1">
       <c r="A13" t="s" s="19">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="B13" t="s" s="20">
         <v>32</v>
@@ -5907,7 +6231,7 @@
     </row>
     <row r="14" ht="16" customHeight="1">
       <c r="A14" t="s" s="19">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="B14" t="s" s="20">
         <v>35</v>
@@ -5934,10 +6258,10 @@
     </row>
     <row r="15" ht="16" customHeight="1">
       <c r="A15" t="s" s="19">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="B15" t="s" s="20">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="17"/>
@@ -5959,7 +6283,7 @@
     </row>
     <row r="16" ht="16" customHeight="1">
       <c r="A16" t="s" s="19">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="B16" t="s" s="20">
         <v>40</v>
@@ -5984,7 +6308,7 @@
     </row>
     <row r="17" ht="16" customHeight="1">
       <c r="A17" t="s" s="19">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="B17" t="s" s="20">
         <v>42</v>
@@ -6009,13 +6333,13 @@
     </row>
     <row r="18" ht="16" customHeight="1">
       <c r="A18" t="s" s="19">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="B18" t="s" s="20">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="C18" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -6036,13 +6360,13 @@
     </row>
     <row r="19" ht="16" customHeight="1">
       <c r="A19" t="s" s="19">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s" s="20">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s" s="19">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -6063,13 +6387,13 @@
     </row>
     <row r="20" ht="16" customHeight="1">
       <c r="A20" t="s" s="19">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="B20" t="s" s="20">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="C20" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -6090,13 +6414,13 @@
     </row>
     <row r="21" ht="16" customHeight="1">
       <c r="A21" t="s" s="19">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="B21" t="s" s="20">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s" s="19">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -6117,13 +6441,13 @@
     </row>
     <row r="22" ht="16" customHeight="1">
       <c r="A22" t="s" s="19">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="B22" t="s" s="20">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -6144,13 +6468,13 @@
     </row>
     <row r="23" ht="16" customHeight="1">
       <c r="A23" t="s" s="19">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="B23" t="s" s="20">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="C23" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -6171,13 +6495,13 @@
     </row>
     <row r="24" ht="16" customHeight="1">
       <c r="A24" t="s" s="19">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="B24" t="s" s="20">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="C24" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -6198,13 +6522,13 @@
     </row>
     <row r="25" ht="16" customHeight="1">
       <c r="A25" t="s" s="19">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="B25" t="s" s="20">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="C25" t="s" s="19">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -6225,13 +6549,13 @@
     </row>
     <row r="26" ht="16" customHeight="1">
       <c r="A26" t="s" s="19">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="B26" t="s" s="20">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="C26" t="s" s="19">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
@@ -6252,13 +6576,13 @@
     </row>
     <row r="27" ht="16" customHeight="1">
       <c r="A27" t="s" s="19">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="B27" t="s" s="20">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="C27" t="s" s="19">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
@@ -6279,13 +6603,13 @@
     </row>
     <row r="28" ht="16" customHeight="1">
       <c r="A28" t="s" s="19">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="B28" t="s" s="20">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="C28" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -6306,13 +6630,13 @@
     </row>
     <row r="29" ht="16" customHeight="1">
       <c r="A29" t="s" s="19">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="B29" t="s" s="20">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="C29" t="s" s="19">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
@@ -6333,13 +6657,13 @@
     </row>
     <row r="30" ht="16" customHeight="1">
       <c r="A30" t="s" s="19">
+        <v>240</v>
+      </c>
+      <c r="B30" t="s" s="20">
+        <v>241</v>
+      </c>
+      <c r="C30" t="s" s="19">
         <v>222</v>
-      </c>
-      <c r="B30" t="s" s="20">
-        <v>223</v>
-      </c>
-      <c r="C30" t="s" s="19">
-        <v>204</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -6360,13 +6684,13 @@
     </row>
     <row r="31" ht="16" customHeight="1">
       <c r="A31" t="s" s="19">
+        <v>242</v>
+      </c>
+      <c r="B31" t="s" s="20">
+        <v>241</v>
+      </c>
+      <c r="C31" t="s" s="19">
         <v>224</v>
-      </c>
-      <c r="B31" t="s" s="20">
-        <v>223</v>
-      </c>
-      <c r="C31" t="s" s="19">
-        <v>206</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
@@ -6387,13 +6711,13 @@
     </row>
     <row r="32" ht="16" customHeight="1">
       <c r="A32" t="s" s="19">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="B32" t="s" s="20">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="C32" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
@@ -6414,13 +6738,13 @@
     </row>
     <row r="33" ht="16" customHeight="1">
       <c r="A33" t="s" s="19">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="B33" t="s" s="20">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="C33" t="s" s="19">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
@@ -6441,13 +6765,13 @@
     </row>
     <row r="34" ht="16" customHeight="1">
       <c r="A34" t="s" s="19">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B34" t="s" s="20">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="C34" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
@@ -6468,13 +6792,13 @@
     </row>
     <row r="35" ht="16" customHeight="1">
       <c r="A35" t="s" s="19">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="B35" t="s" s="20">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="C35" t="s" s="19">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
@@ -6495,13 +6819,13 @@
     </row>
     <row r="36" ht="16" customHeight="1">
       <c r="A36" t="s" s="19">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="B36" t="s" s="20">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="C36" t="s" s="19">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
@@ -6522,13 +6846,13 @@
     </row>
     <row r="37" ht="16" customHeight="1">
       <c r="A37" t="s" s="19">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="B37" t="s" s="20">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="C37" t="s" s="19">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
@@ -6549,13 +6873,13 @@
     </row>
     <row r="38" ht="16" customHeight="1">
       <c r="A38" t="s" s="19">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="B38" t="s" s="20">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="C38" t="s" s="19">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -6576,13 +6900,13 @@
     </row>
     <row r="39" ht="16" customHeight="1">
       <c r="A39" t="s" s="19">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="B39" t="s" s="20">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="C39" t="s" s="19">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
@@ -6603,13 +6927,13 @@
     </row>
     <row r="40" ht="16" customHeight="1">
       <c r="A40" t="s" s="19">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="B40" t="s" s="20">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="C40" t="s" s="19">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
@@ -6630,13 +6954,13 @@
     </row>
     <row r="41" ht="16" customHeight="1">
       <c r="A41" t="s" s="19">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="B41" t="s" s="20">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="C41" t="s" s="19">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
@@ -6657,13 +6981,13 @@
     </row>
     <row r="42" ht="16" customHeight="1">
       <c r="A42" t="s" s="19">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="B42" t="s" s="20">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="C42" t="s" s="19">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
@@ -6684,13 +7008,13 @@
     </row>
     <row r="43" ht="16" customHeight="1">
       <c r="A43" t="s" s="19">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="B43" t="s" s="20">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="C43" t="s" s="19">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
@@ -6711,13 +7035,13 @@
     </row>
     <row r="44" ht="16" customHeight="1">
       <c r="A44" t="s" s="27">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="B44" t="s" s="28">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="C44" t="s" s="27">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
@@ -6738,7 +7062,7 @@
     </row>
     <row r="45" ht="19" customHeight="1">
       <c r="A45" t="s" s="8">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="29"/>
@@ -6782,10 +7106,10 @@
     </row>
     <row r="46" ht="16" customHeight="1">
       <c r="A46" t="s" s="14">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="B46" t="s" s="15">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="17"/>
@@ -6807,7 +7131,7 @@
     </row>
     <row r="47" ht="16" customHeight="1">
       <c r="A47" t="s" s="19">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="B47" t="s" s="20">
         <v>89</v>
@@ -6832,13 +7156,13 @@
     </row>
     <row r="48" ht="16" customHeight="1">
       <c r="A48" t="s" s="19">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B48" t="s" s="20">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="C48" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
@@ -6859,13 +7183,13 @@
     </row>
     <row r="49" ht="16" customHeight="1">
       <c r="A49" t="s" s="19">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="B49" t="s" s="20">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="C49" t="s" s="19">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="D49" s="17"/>
       <c r="E49" s="17"/>
@@ -6886,13 +7210,13 @@
     </row>
     <row r="50" ht="16" customHeight="1">
       <c r="A50" t="s" s="19">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="B50" t="s" s="20">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="C50" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
@@ -6913,13 +7237,13 @@
     </row>
     <row r="51" ht="16" customHeight="1">
       <c r="A51" t="s" s="27">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="B51" t="s" s="28">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="C51" t="s" s="27">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
@@ -6940,7 +7264,7 @@
     </row>
     <row r="52" ht="19" customHeight="1">
       <c r="A52" t="s" s="43">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="44"/>
@@ -6984,7 +7308,7 @@
     </row>
     <row r="53" ht="16" customHeight="1">
       <c r="A53" t="s" s="14">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="B53" t="s" s="15">
         <v>103</v>
@@ -7009,7 +7333,7 @@
     </row>
     <row r="54" ht="16" customHeight="1">
       <c r="A54" t="s" s="19">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="B54" t="s" s="20">
         <v>105</v>
@@ -7034,7 +7358,7 @@
     </row>
     <row r="55" ht="16" customHeight="1">
       <c r="A55" t="s" s="19">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="B55" t="s" s="20">
         <v>107</v>
@@ -7061,10 +7385,10 @@
     </row>
     <row r="56" ht="16" customHeight="1">
       <c r="A56" t="s" s="19">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="B56" t="s" s="20">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="17"/>
@@ -7086,10 +7410,10 @@
     </row>
     <row r="57" ht="16" customHeight="1">
       <c r="A57" t="s" s="19">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="B57" t="s" s="20">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="C57" t="s" s="19">
         <v>14</v>
@@ -7113,7 +7437,7 @@
     </row>
     <row r="58" ht="16" customHeight="1">
       <c r="A58" t="s" s="19">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="B58" t="s" s="20">
         <v>113</v>
@@ -7138,7 +7462,7 @@
     </row>
     <row r="59" ht="16" customHeight="1">
       <c r="A59" t="s" s="33">
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="B59" t="s" s="20">
         <v>115</v>
@@ -7163,7 +7487,7 @@
     </row>
     <row r="60" ht="16" customHeight="1">
       <c r="A60" t="s" s="19">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="B60" t="s" s="20">
         <v>117</v>
@@ -7190,7 +7514,7 @@
     </row>
     <row r="61" ht="16" customHeight="1">
       <c r="A61" t="s" s="19">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="B61" t="s" s="20">
         <v>120</v>
@@ -7217,7 +7541,7 @@
     </row>
     <row r="62" ht="16" customHeight="1">
       <c r="A62" t="s" s="19">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="B62" t="s" s="20">
         <v>123</v>
@@ -7242,7 +7566,7 @@
     </row>
     <row r="63" ht="16" customHeight="1">
       <c r="A63" t="s" s="19">
-        <v>279</v>
+        <v>297</v>
       </c>
       <c r="B63" t="s" s="20">
         <v>125</v>
@@ -7267,7 +7591,7 @@
     </row>
     <row r="64" ht="16" customHeight="1">
       <c r="A64" t="s" s="19">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="B64" t="s" s="20">
         <v>127</v>
@@ -7294,7 +7618,7 @@
     </row>
     <row r="65" ht="16" customHeight="1">
       <c r="A65" t="s" s="19">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="B65" t="s" s="20">
         <v>130</v>
@@ -7319,13 +7643,13 @@
     </row>
     <row r="66" ht="16" customHeight="1">
       <c r="A66" t="s" s="19">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="B66" t="s" s="20">
         <v>132</v>
       </c>
       <c r="C66" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D66" s="17"/>
       <c r="E66" s="17"/>
@@ -7346,13 +7670,13 @@
     </row>
     <row r="67" ht="16" customHeight="1">
       <c r="A67" t="s" s="19">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="B67" t="s" s="20">
         <v>132</v>
       </c>
       <c r="C67" t="s" s="19">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="D67" s="17"/>
       <c r="E67" s="17"/>
@@ -7373,13 +7697,13 @@
     </row>
     <row r="68" ht="16" customHeight="1">
       <c r="A68" t="s" s="19">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="B68" t="s" s="20">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="C68" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D68" s="17"/>
       <c r="E68" s="17"/>
@@ -7400,13 +7724,13 @@
     </row>
     <row r="69" ht="16" customHeight="1">
       <c r="A69" t="s" s="19">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="B69" t="s" s="20">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="C69" t="s" s="19">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D69" s="17"/>
       <c r="E69" s="17"/>
@@ -7427,13 +7751,13 @@
     </row>
     <row r="70" ht="16" customHeight="1">
       <c r="A70" t="s" s="19">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="B70" t="s" s="20">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="C70" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D70" s="17"/>
       <c r="E70" s="17"/>
@@ -7454,13 +7778,13 @@
     </row>
     <row r="71" ht="16" customHeight="1">
       <c r="A71" t="s" s="19">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="B71" t="s" s="20">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="C71" t="s" s="19">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
@@ -7481,13 +7805,13 @@
     </row>
     <row r="72" ht="16" customHeight="1">
       <c r="A72" t="s" s="19">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="B72" t="s" s="20">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="C72" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D72" s="17"/>
       <c r="E72" s="17"/>
@@ -7508,13 +7832,13 @@
     </row>
     <row r="73" ht="16" customHeight="1">
       <c r="A73" t="s" s="19">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="B73" t="s" s="20">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="C73" t="s" s="19">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D73" s="17"/>
       <c r="E73" s="17"/>
@@ -7535,13 +7859,13 @@
     </row>
     <row r="74" ht="16" customHeight="1">
       <c r="A74" t="s" s="19">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="B74" t="s" s="20">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="C74" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
@@ -7562,13 +7886,13 @@
     </row>
     <row r="75" ht="16" customHeight="1">
       <c r="A75" t="s" s="19">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="B75" t="s" s="20">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="C75" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
@@ -7589,13 +7913,13 @@
     </row>
     <row r="76" ht="16" customHeight="1">
       <c r="A76" t="s" s="19">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="B76" t="s" s="20">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="C76" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D76" s="17"/>
       <c r="E76" s="17"/>
@@ -7616,13 +7940,13 @@
     </row>
     <row r="77" ht="16" customHeight="1">
       <c r="A77" t="s" s="19">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="B77" t="s" s="20">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="C77" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
@@ -7643,13 +7967,13 @@
     </row>
     <row r="78" ht="16" customHeight="1">
       <c r="A78" t="s" s="19">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="B78" t="s" s="20">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="C78" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D78" s="17"/>
       <c r="E78" s="17"/>
@@ -7670,13 +7994,13 @@
     </row>
     <row r="79" ht="16" customHeight="1">
       <c r="A79" t="s" s="19">
-        <v>303</v>
+        <v>321</v>
       </c>
       <c r="B79" t="s" s="20">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="C79" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D79" s="17"/>
       <c r="E79" s="17"/>
@@ -7697,13 +8021,13 @@
     </row>
     <row r="80" ht="16" customHeight="1">
       <c r="A80" t="s" s="19">
-        <v>305</v>
+        <v>323</v>
       </c>
       <c r="B80" t="s" s="20">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="C80" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D80" s="17"/>
       <c r="E80" s="17"/>
@@ -7724,13 +8048,13 @@
     </row>
     <row r="81" ht="16" customHeight="1">
       <c r="A81" t="s" s="19">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="B81" t="s" s="20">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="C81" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D81" s="17"/>
       <c r="E81" s="17"/>
@@ -7751,13 +8075,13 @@
     </row>
     <row r="82" ht="16" customHeight="1">
       <c r="A82" t="s" s="19">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="B82" t="s" s="20">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="C82" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D82" s="17"/>
       <c r="E82" s="17"/>
@@ -7778,13 +8102,13 @@
     </row>
     <row r="83" ht="16" customHeight="1">
       <c r="A83" t="s" s="19">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="B83" t="s" s="20">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="C83" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D83" s="17"/>
       <c r="E83" s="17"/>
@@ -7805,13 +8129,13 @@
     </row>
     <row r="84" ht="16" customHeight="1">
       <c r="A84" t="s" s="19">
-        <v>313</v>
+        <v>331</v>
       </c>
       <c r="B84" t="s" s="20">
-        <v>314</v>
+        <v>332</v>
       </c>
       <c r="C84" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D84" s="17"/>
       <c r="E84" s="17"/>
@@ -7832,13 +8156,13 @@
     </row>
     <row r="85" ht="16" customHeight="1">
       <c r="A85" t="s" s="19">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="B85" t="s" s="20">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="C85" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D85" s="17"/>
       <c r="E85" s="17"/>
@@ -7859,13 +8183,13 @@
     </row>
     <row r="86" ht="16" customHeight="1">
       <c r="A86" t="s" s="19">
-        <v>317</v>
+        <v>335</v>
       </c>
       <c r="B86" t="s" s="20">
         <v>156</v>
       </c>
       <c r="C86" t="s" s="19">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="D86" s="17"/>
       <c r="E86" s="17"/>
@@ -7886,13 +8210,13 @@
     </row>
     <row r="87" ht="16" customHeight="1">
       <c r="A87" t="s" s="19">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="B87" t="s" s="20">
-        <v>319</v>
+        <v>337</v>
       </c>
       <c r="C87" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D87" s="17"/>
       <c r="E87" s="17"/>
@@ -7913,13 +8237,13 @@
     </row>
     <row r="88" ht="16" customHeight="1">
       <c r="A88" t="s" s="19">
-        <v>320</v>
+        <v>338</v>
       </c>
       <c r="B88" t="s" s="20">
-        <v>321</v>
+        <v>339</v>
       </c>
       <c r="C88" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D88" s="17"/>
       <c r="E88" s="17"/>
@@ -7940,13 +8264,13 @@
     </row>
     <row r="89" ht="16" customHeight="1">
       <c r="A89" t="s" s="19">
-        <v>322</v>
+        <v>340</v>
       </c>
       <c r="B89" t="s" s="20">
-        <v>323</v>
+        <v>341</v>
       </c>
       <c r="C89" t="s" s="19">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="D89" s="17"/>
       <c r="E89" s="17"/>
@@ -7967,13 +8291,13 @@
     </row>
     <row r="90" ht="16" customHeight="1">
       <c r="A90" t="s" s="19">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="B90" t="s" s="20">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="C90" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D90" s="17"/>
       <c r="E90" s="17"/>
@@ -7994,13 +8318,13 @@
     </row>
     <row r="91" ht="16" customHeight="1">
       <c r="A91" t="s" s="19">
-        <v>326</v>
+        <v>344</v>
       </c>
       <c r="B91" t="s" s="20">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="C91" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D91" s="17"/>
       <c r="E91" s="17"/>
@@ -8021,13 +8345,13 @@
     </row>
     <row r="92" ht="16" customHeight="1">
       <c r="A92" t="s" s="19">
-        <v>328</v>
+        <v>346</v>
       </c>
       <c r="B92" t="s" s="20">
-        <v>329</v>
+        <v>347</v>
       </c>
       <c r="C92" t="s" s="19">
-        <v>199</v>
+        <v>348</v>
       </c>
       <c r="D92" s="17"/>
       <c r="E92" s="17"/>
@@ -8048,13 +8372,13 @@
     </row>
     <row r="93" ht="16" customHeight="1">
       <c r="A93" t="s" s="19">
-        <v>330</v>
+        <v>349</v>
       </c>
       <c r="B93" t="s" s="20">
-        <v>331</v>
+        <v>350</v>
       </c>
       <c r="C93" t="s" s="19">
-        <v>204</v>
+        <v>351</v>
       </c>
       <c r="D93" s="17"/>
       <c r="E93" s="17"/>
@@ -8075,13 +8399,13 @@
     </row>
     <row r="94" ht="16" customHeight="1">
       <c r="A94" t="s" s="19">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="B94" t="s" s="20">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="C94" t="s" s="19">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D94" s="17"/>
       <c r="E94" s="17"/>
@@ -8102,13 +8426,13 @@
     </row>
     <row r="95" ht="16" customHeight="1">
       <c r="A95" t="s" s="19">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="B95" t="s" s="20">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="C95" t="s" s="19">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D95" s="17"/>
       <c r="E95" s="17"/>
@@ -8129,13 +8453,13 @@
     </row>
     <row r="96" ht="16" customHeight="1">
       <c r="A96" t="s" s="19">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="B96" t="s" s="20">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="C96" t="s" s="19">
-        <v>199</v>
+        <v>348</v>
       </c>
       <c r="D96" s="17"/>
       <c r="E96" s="17"/>
@@ -8156,13 +8480,13 @@
     </row>
     <row r="97" ht="16" customHeight="1">
       <c r="A97" t="s" s="19">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="B97" t="s" s="20">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="C97" t="s" s="19">
-        <v>204</v>
+        <v>351</v>
       </c>
       <c r="D97" s="17"/>
       <c r="E97" s="17"/>
@@ -8182,40 +8506,256 @@
       </c>
     </row>
     <row r="98" ht="16" customHeight="1">
-      <c r="A98" s="21"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="21"/>
+      <c r="A98" t="s" s="19">
+        <v>360</v>
+      </c>
+      <c r="B98" t="s" s="20">
+        <v>361</v>
+      </c>
+      <c r="C98" t="s" s="19">
+        <v>217</v>
+      </c>
       <c r="D98" s="17"/>
       <c r="E98" s="17"/>
       <c r="F98" s="17"/>
       <c r="G98" s="17"/>
       <c r="H98" s="17"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="17"/>
+      <c r="I98" s="24"/>
+      <c r="J98" s="25"/>
+      <c r="K98" s="25"/>
+      <c r="L98" s="26"/>
       <c r="M98" s="17"/>
       <c r="N98" s="17"/>
       <c r="O98" s="17"/>
-      <c r="P98" s="17"/>
+      <c r="P98" s="18">
+        <f>SUM(D98:O98)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="99" ht="16" customHeight="1">
-      <c r="A99" s="21"/>
-      <c r="B99" s="17"/>
-      <c r="C99" s="21"/>
+      <c r="A99" t="s" s="19">
+        <v>362</v>
+      </c>
+      <c r="B99" t="s" s="20">
+        <v>363</v>
+      </c>
+      <c r="C99" t="s" s="19">
+        <v>222</v>
+      </c>
       <c r="D99" s="17"/>
       <c r="E99" s="17"/>
       <c r="F99" s="17"/>
       <c r="G99" s="17"/>
       <c r="H99" s="17"/>
-      <c r="I99" s="17"/>
-      <c r="J99" s="17"/>
-      <c r="K99" s="17"/>
-      <c r="L99" s="17"/>
+      <c r="I99" s="24"/>
+      <c r="J99" s="25"/>
+      <c r="K99" s="25"/>
+      <c r="L99" s="26"/>
       <c r="M99" s="17"/>
       <c r="N99" s="17"/>
       <c r="O99" s="17"/>
-      <c r="P99" s="17"/>
+      <c r="P99" s="18">
+        <f>SUM(D99:O99)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" ht="16" customHeight="1">
+      <c r="A100" t="s" s="19">
+        <v>364</v>
+      </c>
+      <c r="B100" t="s" s="20">
+        <v>365</v>
+      </c>
+      <c r="C100" t="s" s="19">
+        <v>348</v>
+      </c>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="24"/>
+      <c r="J100" s="25"/>
+      <c r="K100" s="25"/>
+      <c r="L100" s="26"/>
+      <c r="M100" s="17"/>
+      <c r="N100" s="17"/>
+      <c r="O100" s="17"/>
+      <c r="P100" s="18">
+        <f>SUM(D100:O100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" ht="16" customHeight="1">
+      <c r="A101" t="s" s="19">
+        <v>366</v>
+      </c>
+      <c r="B101" t="s" s="20">
+        <v>367</v>
+      </c>
+      <c r="C101" t="s" s="19">
+        <v>351</v>
+      </c>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="24"/>
+      <c r="J101" s="25"/>
+      <c r="K101" s="25"/>
+      <c r="L101" s="26"/>
+      <c r="M101" s="17"/>
+      <c r="N101" s="17"/>
+      <c r="O101" s="17"/>
+      <c r="P101" s="18">
+        <f>SUM(D101:O101)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" ht="16" customHeight="1">
+      <c r="A102" t="s" s="19">
+        <v>368</v>
+      </c>
+      <c r="B102" t="s" s="20">
+        <v>369</v>
+      </c>
+      <c r="C102" t="s" s="19">
+        <v>217</v>
+      </c>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="25"/>
+      <c r="K102" s="25"/>
+      <c r="L102" s="26"/>
+      <c r="M102" s="17"/>
+      <c r="N102" s="17"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="18">
+        <f>SUM(D102:O102)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" ht="16" customHeight="1">
+      <c r="A103" t="s" s="19">
+        <v>370</v>
+      </c>
+      <c r="B103" t="s" s="20">
+        <v>371</v>
+      </c>
+      <c r="C103" t="s" s="19">
+        <v>222</v>
+      </c>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="24"/>
+      <c r="J103" s="25"/>
+      <c r="K103" s="25"/>
+      <c r="L103" s="26"/>
+      <c r="M103" s="17"/>
+      <c r="N103" s="17"/>
+      <c r="O103" s="17"/>
+      <c r="P103" s="18">
+        <f>SUM(D103:O103)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" ht="16" customHeight="1">
+      <c r="A104" t="s" s="19">
+        <v>372</v>
+      </c>
+      <c r="B104" t="s" s="20">
+        <v>373</v>
+      </c>
+      <c r="C104" t="s" s="19">
+        <v>348</v>
+      </c>
+      <c r="D104" s="17"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="17"/>
+      <c r="I104" s="24"/>
+      <c r="J104" s="25"/>
+      <c r="K104" s="25"/>
+      <c r="L104" s="26"/>
+      <c r="M104" s="17"/>
+      <c r="N104" s="17"/>
+      <c r="O104" s="17"/>
+      <c r="P104" s="18">
+        <f>SUM(D104:O104)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" ht="16" customHeight="1">
+      <c r="A105" t="s" s="19">
+        <v>374</v>
+      </c>
+      <c r="B105" t="s" s="20">
+        <v>375</v>
+      </c>
+      <c r="C105" t="s" s="19">
+        <v>351</v>
+      </c>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="17"/>
+      <c r="H105" s="17"/>
+      <c r="I105" s="24"/>
+      <c r="J105" s="25"/>
+      <c r="K105" s="25"/>
+      <c r="L105" s="26"/>
+      <c r="M105" s="17"/>
+      <c r="N105" s="17"/>
+      <c r="O105" s="17"/>
+      <c r="P105" s="18">
+        <f>SUM(D105:O105)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" ht="16" customHeight="1">
+      <c r="A106" s="21"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="17"/>
+      <c r="H106" s="17"/>
+      <c r="I106" s="17"/>
+      <c r="J106" s="13"/>
+      <c r="K106" s="13"/>
+      <c r="L106" s="17"/>
+      <c r="M106" s="17"/>
+      <c r="N106" s="17"/>
+      <c r="O106" s="17"/>
+      <c r="P106" s="17"/>
+    </row>
+    <row r="107" ht="16" customHeight="1">
+      <c r="A107" s="21"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="17"/>
+      <c r="H107" s="17"/>
+      <c r="I107" s="17"/>
+      <c r="J107" s="17"/>
+      <c r="K107" s="17"/>
+      <c r="L107" s="17"/>
+      <c r="M107" s="17"/>
+      <c r="N107" s="17"/>
+      <c r="O107" s="17"/>
+      <c r="P107" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8271,7 +8811,7 @@
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -8303,13 +8843,13 @@
     </row>
     <row r="3" ht="16" customHeight="1">
       <c r="A3" t="s" s="49">
-        <v>340</v>
+        <v>376</v>
       </c>
       <c r="B3" t="s" s="50">
-        <v>341</v>
+        <v>377</v>
       </c>
       <c r="C3" t="s" s="50">
-        <v>342</v>
+        <v>378</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -8326,7 +8866,7 @@
     </row>
     <row r="4" ht="19" customHeight="1">
       <c r="A4" t="s" s="8">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="29"/>
@@ -8358,10 +8898,10 @@
     </row>
     <row r="5" ht="16" customHeight="1">
       <c r="A5" t="s" s="14">
-        <v>343</v>
+        <v>379</v>
       </c>
       <c r="B5" t="s" s="15">
-        <v>344</v>
+        <v>380</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
@@ -8379,10 +8919,10 @@
     </row>
     <row r="6" ht="16" customHeight="1">
       <c r="A6" t="s" s="19">
-        <v>345</v>
+        <v>381</v>
       </c>
       <c r="B6" t="s" s="20">
-        <v>346</v>
+        <v>382</v>
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="17"/>
@@ -8400,10 +8940,10 @@
     </row>
     <row r="7" ht="16" customHeight="1">
       <c r="A7" t="s" s="19">
-        <v>347</v>
+        <v>383</v>
       </c>
       <c r="B7" t="s" s="20">
-        <v>348</v>
+        <v>384</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="17"/>
@@ -8421,10 +8961,10 @@
     </row>
     <row r="8" ht="16" customHeight="1">
       <c r="A8" t="s" s="19">
-        <v>349</v>
+        <v>385</v>
       </c>
       <c r="B8" t="s" s="20">
-        <v>350</v>
+        <v>386</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="17"/>
@@ -8442,13 +8982,13 @@
     </row>
     <row r="9" ht="16" customHeight="1">
       <c r="A9" t="s" s="19">
-        <v>351</v>
+        <v>387</v>
       </c>
       <c r="B9" t="s" s="20">
-        <v>352</v>
+        <v>388</v>
       </c>
       <c r="C9" t="s" s="19">
-        <v>342</v>
+        <v>378</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -8465,13 +9005,13 @@
     </row>
     <row r="10" ht="16" customHeight="1">
       <c r="A10" t="s" s="19">
-        <v>353</v>
+        <v>389</v>
       </c>
       <c r="B10" t="s" s="20">
-        <v>354</v>
+        <v>390</v>
       </c>
       <c r="C10" t="s" s="19">
-        <v>342</v>
+        <v>378</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -8488,13 +9028,13 @@
     </row>
     <row r="11" ht="16" customHeight="1">
       <c r="A11" t="s" s="19">
-        <v>355</v>
+        <v>391</v>
       </c>
       <c r="B11" t="s" s="20">
-        <v>356</v>
+        <v>392</v>
       </c>
       <c r="C11" t="s" s="19">
-        <v>342</v>
+        <v>378</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -8511,13 +9051,13 @@
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" t="s" s="27">
-        <v>357</v>
+        <v>393</v>
       </c>
       <c r="B12" t="s" s="28">
-        <v>358</v>
+        <v>394</v>
       </c>
       <c r="C12" t="s" s="27">
-        <v>342</v>
+        <v>378</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -8534,7 +9074,7 @@
     </row>
     <row r="13" ht="19" customHeight="1">
       <c r="A13" t="s" s="43">
-        <v>359</v>
+        <v>395</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="44"/>
@@ -8566,10 +9106,10 @@
     </row>
     <row r="14" ht="16" customHeight="1">
       <c r="A14" t="s" s="14">
-        <v>360</v>
+        <v>396</v>
       </c>
       <c r="B14" t="s" s="15">
-        <v>361</v>
+        <v>397</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="17"/>
@@ -8587,13 +9127,13 @@
     </row>
     <row r="15" ht="16" customHeight="1">
       <c r="A15" t="s" s="19">
-        <v>362</v>
+        <v>398</v>
       </c>
       <c r="B15" t="s" s="20">
-        <v>363</v>
+        <v>399</v>
       </c>
       <c r="C15" t="s" s="19">
-        <v>364</v>
+        <v>400</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -8610,13 +9150,13 @@
     </row>
     <row r="16" ht="16" customHeight="1">
       <c r="A16" t="s" s="19">
-        <v>365</v>
+        <v>401</v>
       </c>
       <c r="B16" t="s" s="20">
-        <v>366</v>
+        <v>402</v>
       </c>
       <c r="C16" t="s" s="19">
-        <v>367</v>
+        <v>403</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
@@ -8633,10 +9173,10 @@
     </row>
     <row r="17" ht="16" customHeight="1">
       <c r="A17" t="s" s="19">
-        <v>368</v>
+        <v>404</v>
       </c>
       <c r="B17" t="s" s="20">
-        <v>369</v>
+        <v>405</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="17"/>
@@ -8654,10 +9194,10 @@
     </row>
     <row r="18" ht="16" customHeight="1">
       <c r="A18" t="s" s="19">
-        <v>370</v>
+        <v>406</v>
       </c>
       <c r="B18" t="s" s="20">
-        <v>371</v>
+        <v>407</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="17"/>
@@ -8675,10 +9215,10 @@
     </row>
     <row r="19" ht="16" customHeight="1">
       <c r="A19" t="s" s="19">
-        <v>372</v>
+        <v>408</v>
       </c>
       <c r="B19" t="s" s="20">
-        <v>373</v>
+        <v>409</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="17"/>
@@ -8696,10 +9236,10 @@
     </row>
     <row r="20" ht="16" customHeight="1">
       <c r="A20" t="s" s="19">
-        <v>374</v>
+        <v>410</v>
       </c>
       <c r="B20" t="s" s="20">
-        <v>375</v>
+        <v>411</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="17"/>
@@ -8717,13 +9257,13 @@
     </row>
     <row r="21" ht="16" customHeight="1">
       <c r="A21" t="s" s="19">
-        <v>376</v>
+        <v>412</v>
       </c>
       <c r="B21" t="s" s="20">
-        <v>377</v>
+        <v>413</v>
       </c>
       <c r="C21" t="s" s="19">
-        <v>378</v>
+        <v>414</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -8740,13 +9280,13 @@
     </row>
     <row r="22" ht="16" customHeight="1">
       <c r="A22" t="s" s="19">
-        <v>379</v>
+        <v>415</v>
       </c>
       <c r="B22" t="s" s="20">
-        <v>380</v>
+        <v>416</v>
       </c>
       <c r="C22" t="s" s="19">
-        <v>378</v>
+        <v>414</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -8763,13 +9303,13 @@
     </row>
     <row r="23" ht="16" customHeight="1">
       <c r="A23" t="s" s="19">
-        <v>381</v>
+        <v>417</v>
       </c>
       <c r="B23" t="s" s="20">
-        <v>382</v>
+        <v>418</v>
       </c>
       <c r="C23" t="s" s="19">
-        <v>342</v>
+        <v>378</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -8786,13 +9326,13 @@
     </row>
     <row r="24" ht="16" customHeight="1">
       <c r="A24" t="s" s="19">
-        <v>383</v>
+        <v>419</v>
       </c>
       <c r="B24" t="s" s="20">
-        <v>384</v>
+        <v>420</v>
       </c>
       <c r="C24" t="s" s="19">
-        <v>378</v>
+        <v>414</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -8809,13 +9349,13 @@
     </row>
     <row r="25" ht="16" customHeight="1">
       <c r="A25" t="s" s="19">
-        <v>385</v>
+        <v>421</v>
       </c>
       <c r="B25" t="s" s="20">
-        <v>386</v>
+        <v>422</v>
       </c>
       <c r="C25" t="s" s="19">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -8832,10 +9372,10 @@
     </row>
     <row r="26" ht="16" customHeight="1">
       <c r="A26" t="s" s="19">
-        <v>387</v>
+        <v>423</v>
       </c>
       <c r="B26" t="s" s="20">
-        <v>388</v>
+        <v>424</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="17"/>
@@ -8853,10 +9393,10 @@
     </row>
     <row r="27" ht="16" customHeight="1">
       <c r="A27" t="s" s="19">
-        <v>389</v>
+        <v>425</v>
       </c>
       <c r="B27" t="s" s="20">
-        <v>390</v>
+        <v>426</v>
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="17"/>
@@ -8874,10 +9414,10 @@
     </row>
     <row r="28" ht="16" customHeight="1">
       <c r="A28" t="s" s="19">
-        <v>391</v>
+        <v>427</v>
       </c>
       <c r="B28" t="s" s="20">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="17"/>
@@ -10425,7 +10965,7 @@
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="58">
-        <v>393</v>
+        <v>429</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -11445,13 +11985,13 @@
     </row>
     <row r="3" ht="16" customHeight="1">
       <c r="A3" t="s" s="14">
-        <v>394</v>
+        <v>430</v>
       </c>
       <c r="B3" t="s" s="15">
-        <v>395</v>
+        <v>431</v>
       </c>
       <c r="C3" t="s" s="15">
-        <v>396</v>
+        <v>432</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -12456,10 +12996,10 @@
     </row>
     <row r="4" ht="16" customHeight="1">
       <c r="A4" t="s" s="19">
-        <v>397</v>
+        <v>433</v>
       </c>
       <c r="B4" t="s" s="59">
-        <v>398</v>
+        <v>434</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="17"/>
@@ -13465,10 +14005,10 @@
     </row>
     <row r="5" ht="16" customHeight="1">
       <c r="A5" t="s" s="19">
-        <v>399</v>
+        <v>435</v>
       </c>
       <c r="B5" t="s" s="59">
-        <v>400</v>
+        <v>436</v>
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="17"/>
@@ -14474,10 +15014,10 @@
     </row>
     <row r="6" ht="16" customHeight="1">
       <c r="A6" t="s" s="19">
-        <v>401</v>
+        <v>437</v>
       </c>
       <c r="B6" t="s" s="59">
-        <v>402</v>
+        <v>438</v>
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="17"/>
@@ -15483,10 +16023,10 @@
     </row>
     <row r="7" ht="16" customHeight="1">
       <c r="A7" t="s" s="19">
-        <v>403</v>
+        <v>439</v>
       </c>
       <c r="B7" t="s" s="59">
-        <v>404</v>
+        <v>440</v>
       </c>
       <c r="C7" s="60"/>
       <c r="D7" s="17"/>
@@ -16492,10 +17032,10 @@
     </row>
     <row r="8" ht="16" customHeight="1">
       <c r="A8" t="s" s="19">
-        <v>405</v>
+        <v>441</v>
       </c>
       <c r="B8" t="s" s="59">
-        <v>406</v>
+        <v>442</v>
       </c>
       <c r="C8" s="60"/>
       <c r="D8" s="17"/>
@@ -17501,10 +18041,10 @@
     </row>
     <row r="9" ht="16" customHeight="1">
       <c r="A9" t="s" s="19">
-        <v>407</v>
+        <v>443</v>
       </c>
       <c r="B9" t="s" s="59">
-        <v>408</v>
+        <v>444</v>
       </c>
       <c r="C9" s="60"/>
       <c r="D9" s="17"/>
@@ -18510,10 +19050,10 @@
     </row>
     <row r="10" ht="16" customHeight="1">
       <c r="A10" t="s" s="27">
-        <v>409</v>
+        <v>445</v>
       </c>
       <c r="B10" t="s" s="61">
-        <v>410</v>
+        <v>446</v>
       </c>
       <c r="C10" s="62"/>
       <c r="D10" s="17"/>
@@ -19519,7 +20059,7 @@
     </row>
     <row r="11" ht="19" customHeight="1">
       <c r="A11" t="s" s="58">
-        <v>411</v>
+        <v>447</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -20523,10 +21063,10 @@
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" t="s" s="14">
-        <v>412</v>
+        <v>448</v>
       </c>
       <c r="B12" t="s" s="15">
-        <v>413</v>
+        <v>449</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="17"/>
@@ -21532,10 +22072,10 @@
     </row>
     <row r="13" ht="16" customHeight="1">
       <c r="A13" t="s" s="19">
-        <v>414</v>
+        <v>450</v>
       </c>
       <c r="B13" t="s" s="20">
-        <v>415</v>
+        <v>451</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -22541,10 +23081,10 @@
     </row>
     <row r="14" ht="16" customHeight="1">
       <c r="A14" t="s" s="19">
-        <v>416</v>
+        <v>452</v>
       </c>
       <c r="B14" t="s" s="20">
-        <v>417</v>
+        <v>453</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -23550,10 +24090,10 @@
     </row>
     <row r="15" ht="16" customHeight="1">
       <c r="A15" t="s" s="33">
-        <v>418</v>
+        <v>454</v>
       </c>
       <c r="B15" t="s" s="59">
-        <v>419</v>
+        <v>455</v>
       </c>
       <c r="C15" s="60"/>
       <c r="D15" s="17"/>
@@ -24559,10 +25099,10 @@
     </row>
     <row r="16" ht="16" customHeight="1">
       <c r="A16" t="s" s="19">
-        <v>420</v>
+        <v>456</v>
       </c>
       <c r="B16" t="s" s="59">
-        <v>421</v>
+        <v>457</v>
       </c>
       <c r="C16" s="60"/>
       <c r="D16" s="17"/>
@@ -25568,10 +26108,10 @@
     </row>
     <row r="17" ht="16" customHeight="1">
       <c r="A17" t="s" s="33">
-        <v>422</v>
+        <v>458</v>
       </c>
       <c r="B17" t="s" s="59">
-        <v>423</v>
+        <v>459</v>
       </c>
       <c r="C17" s="60"/>
       <c r="D17" s="17"/>
@@ -26577,13 +27117,13 @@
     </row>
     <row r="18" ht="16" customHeight="1">
       <c r="A18" t="s" s="19">
-        <v>424</v>
+        <v>460</v>
       </c>
       <c r="B18" t="s" s="59">
-        <v>425</v>
+        <v>461</v>
       </c>
       <c r="C18" t="s" s="59">
-        <v>396</v>
+        <v>432</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -27588,10 +28128,10 @@
     </row>
     <row r="19" ht="16" customHeight="1">
       <c r="A19" t="s" s="19">
-        <v>426</v>
+        <v>462</v>
       </c>
       <c r="B19" t="s" s="20">
-        <v>427</v>
+        <v>463</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -28597,10 +29137,10 @@
     </row>
     <row r="20" ht="16" customHeight="1">
       <c r="A20" t="s" s="19">
-        <v>428</v>
+        <v>464</v>
       </c>
       <c r="B20" t="s" s="20">
-        <v>429</v>
+        <v>465</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -30608,7 +31148,7 @@
     </row>
     <row r="22" ht="19" customHeight="1">
       <c r="A22" t="s" s="58">
-        <v>430</v>
+        <v>466</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -31628,13 +32168,13 @@
     </row>
     <row r="23" ht="16" customHeight="1">
       <c r="A23" t="s" s="14">
+        <v>467</v>
+      </c>
+      <c r="B23" t="s" s="15">
         <v>431</v>
       </c>
-      <c r="B23" t="s" s="15">
-        <v>395</v>
-      </c>
       <c r="C23" t="s" s="15">
-        <v>396</v>
+        <v>432</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -32639,10 +33179,10 @@
     </row>
     <row r="24" ht="16" customHeight="1">
       <c r="A24" t="s" s="19">
-        <v>432</v>
+        <v>468</v>
       </c>
       <c r="B24" t="s" s="59">
-        <v>398</v>
+        <v>434</v>
       </c>
       <c r="C24" s="60"/>
       <c r="D24" s="17"/>
@@ -33648,10 +34188,10 @@
     </row>
     <row r="25" ht="16" customHeight="1">
       <c r="A25" t="s" s="19">
-        <v>433</v>
+        <v>469</v>
       </c>
       <c r="B25" t="s" s="59">
-        <v>400</v>
+        <v>436</v>
       </c>
       <c r="C25" s="60"/>
       <c r="D25" s="17"/>
@@ -34657,10 +35197,10 @@
     </row>
     <row r="26" ht="16" customHeight="1">
       <c r="A26" t="s" s="19">
-        <v>434</v>
+        <v>470</v>
       </c>
       <c r="B26" t="s" s="59">
-        <v>402</v>
+        <v>438</v>
       </c>
       <c r="C26" s="60"/>
       <c r="D26" s="17"/>
@@ -35666,10 +36206,10 @@
     </row>
     <row r="27" ht="16" customHeight="1">
       <c r="A27" t="s" s="19">
-        <v>435</v>
+        <v>471</v>
       </c>
       <c r="B27" t="s" s="59">
-        <v>404</v>
+        <v>440</v>
       </c>
       <c r="C27" s="60"/>
       <c r="D27" s="17"/>
@@ -36675,10 +37215,10 @@
     </row>
     <row r="28" ht="16" customHeight="1">
       <c r="A28" t="s" s="19">
-        <v>436</v>
+        <v>472</v>
       </c>
       <c r="B28" t="s" s="59">
-        <v>406</v>
+        <v>442</v>
       </c>
       <c r="C28" s="60"/>
       <c r="D28" s="17"/>
@@ -37684,10 +38224,10 @@
     </row>
     <row r="29" ht="16" customHeight="1">
       <c r="A29" t="s" s="19">
-        <v>437</v>
+        <v>473</v>
       </c>
       <c r="B29" t="s" s="59">
-        <v>408</v>
+        <v>444</v>
       </c>
       <c r="C29" s="60"/>
       <c r="D29" s="17"/>
@@ -38693,10 +39233,10 @@
     </row>
     <row r="30" ht="16" customHeight="1">
       <c r="A30" t="s" s="27">
-        <v>438</v>
+        <v>474</v>
       </c>
       <c r="B30" t="s" s="61">
-        <v>410</v>
+        <v>446</v>
       </c>
       <c r="C30" s="62"/>
       <c r="D30" s="17"/>
@@ -39702,7 +40242,7 @@
     </row>
     <row r="31" ht="19" customHeight="1">
       <c r="A31" t="s" s="58">
-        <v>439</v>
+        <v>475</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -40706,10 +41246,10 @@
     </row>
     <row r="32" ht="16" customHeight="1">
       <c r="A32" t="s" s="14">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="B32" t="s" s="15">
-        <v>413</v>
+        <v>449</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="17"/>
@@ -41715,10 +42255,10 @@
     </row>
     <row r="33" ht="16" customHeight="1">
       <c r="A33" t="s" s="19">
-        <v>441</v>
+        <v>477</v>
       </c>
       <c r="B33" t="s" s="20">
-        <v>415</v>
+        <v>451</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -42724,10 +43264,10 @@
     </row>
     <row r="34" ht="16" customHeight="1">
       <c r="A34" t="s" s="19">
-        <v>442</v>
+        <v>478</v>
       </c>
       <c r="B34" t="s" s="20">
-        <v>417</v>
+        <v>453</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -43733,10 +44273,10 @@
     </row>
     <row r="35" ht="16" customHeight="1">
       <c r="A35" t="s" s="33">
-        <v>443</v>
+        <v>479</v>
       </c>
       <c r="B35" t="s" s="59">
-        <v>419</v>
+        <v>455</v>
       </c>
       <c r="C35" s="60"/>
       <c r="D35" s="17"/>
@@ -44742,10 +45282,10 @@
     </row>
     <row r="36" ht="16" customHeight="1">
       <c r="A36" t="s" s="19">
-        <v>444</v>
+        <v>480</v>
       </c>
       <c r="B36" t="s" s="59">
-        <v>421</v>
+        <v>457</v>
       </c>
       <c r="C36" s="60"/>
       <c r="D36" s="17"/>
@@ -45751,10 +46291,10 @@
     </row>
     <row r="37" ht="16" customHeight="1">
       <c r="A37" t="s" s="33">
-        <v>445</v>
+        <v>481</v>
       </c>
       <c r="B37" t="s" s="59">
-        <v>423</v>
+        <v>459</v>
       </c>
       <c r="C37" s="60"/>
       <c r="D37" s="17"/>
@@ -46760,13 +47300,13 @@
     </row>
     <row r="38" ht="16" customHeight="1">
       <c r="A38" t="s" s="19">
-        <v>446</v>
+        <v>482</v>
       </c>
       <c r="B38" t="s" s="59">
-        <v>425</v>
+        <v>461</v>
       </c>
       <c r="C38" t="s" s="59">
-        <v>396</v>
+        <v>432</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -47771,10 +48311,10 @@
     </row>
     <row r="39" ht="16" customHeight="1">
       <c r="A39" t="s" s="19">
-        <v>447</v>
+        <v>483</v>
       </c>
       <c r="B39" t="s" s="20">
-        <v>427</v>
+        <v>463</v>
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -48780,10 +49320,10 @@
     </row>
     <row r="40" ht="16" customHeight="1">
       <c r="A40" t="s" s="19">
-        <v>448</v>
+        <v>484</v>
       </c>
       <c r="B40" t="s" s="20">
-        <v>429</v>
+        <v>465</v>
       </c>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -52906,7 +53446,7 @@
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="43">
-        <v>449</v>
+        <v>485</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -52936,7 +53476,7 @@
     <row r="3" ht="19" customHeight="1">
       <c r="A3" s="76"/>
       <c r="B3" t="s" s="77">
-        <v>450</v>
+        <v>486</v>
       </c>
       <c r="C3" t="s" s="78">
         <v>2</v>
@@ -52954,10 +53494,10 @@
     </row>
     <row r="4" ht="16" customHeight="1">
       <c r="A4" t="s" s="80">
-        <v>451</v>
+        <v>487</v>
       </c>
       <c r="B4" t="s" s="81">
-        <v>452</v>
+        <v>488</v>
       </c>
       <c r="C4" s="82"/>
       <c r="D4" s="69"/>
@@ -52977,7 +53517,7 @@
     <row r="5" ht="16" customHeight="1">
       <c r="A5" s="84"/>
       <c r="B5" t="s" s="85">
-        <v>453</v>
+        <v>489</v>
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="69"/>
@@ -52993,10 +53533,10 @@
     </row>
     <row r="6" ht="16" customHeight="1">
       <c r="A6" t="s" s="80">
-        <v>454</v>
+        <v>490</v>
       </c>
       <c r="B6" t="s" s="81">
-        <v>455</v>
+        <v>491</v>
       </c>
       <c r="C6" s="82"/>
       <c r="D6" s="69"/>
@@ -53016,7 +53556,7 @@
     <row r="7" ht="16" customHeight="1">
       <c r="A7" s="82"/>
       <c r="B7" t="s" s="85">
-        <v>456</v>
+        <v>492</v>
       </c>
       <c r="C7" s="82"/>
       <c r="D7" s="69"/>
@@ -53032,10 +53572,10 @@
     </row>
     <row r="8" ht="16" customHeight="1">
       <c r="A8" t="s" s="80">
-        <v>457</v>
+        <v>493</v>
       </c>
       <c r="B8" t="s" s="81">
-        <v>458</v>
+        <v>494</v>
       </c>
       <c r="C8" s="82"/>
       <c r="D8" s="69"/>
@@ -53069,7 +53609,7 @@
     </row>
     <row r="10" ht="19" customHeight="1">
       <c r="A10" t="s" s="43">
-        <v>459</v>
+        <v>495</v>
       </c>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -53087,7 +53627,7 @@
     <row r="11" ht="16" customHeight="1">
       <c r="A11" s="90"/>
       <c r="B11" t="s" s="78">
-        <v>460</v>
+        <v>496</v>
       </c>
       <c r="C11" t="s" s="91">
         <v>2</v>
@@ -53105,10 +53645,10 @@
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" t="s" s="80">
-        <v>461</v>
+        <v>497</v>
       </c>
       <c r="B12" t="s" s="81">
-        <v>462</v>
+        <v>498</v>
       </c>
       <c r="C12" s="82"/>
       <c r="D12" s="69"/>
@@ -53127,10 +53667,10 @@
     </row>
     <row r="13" ht="16" customHeight="1">
       <c r="A13" t="s" s="80">
-        <v>463</v>
+        <v>499</v>
       </c>
       <c r="B13" t="s" s="81">
-        <v>464</v>
+        <v>500</v>
       </c>
       <c r="C13" s="82"/>
       <c r="D13" s="69"/>
@@ -53149,10 +53689,10 @@
     </row>
     <row r="14" ht="16" customHeight="1">
       <c r="A14" t="s" s="80">
-        <v>465</v>
+        <v>501</v>
       </c>
       <c r="B14" t="s" s="81">
-        <v>466</v>
+        <v>502</v>
       </c>
       <c r="C14" s="82"/>
       <c r="D14" s="69"/>
@@ -53172,7 +53712,7 @@
     <row r="15" ht="16" customHeight="1">
       <c r="A15" s="92"/>
       <c r="B15" t="s" s="85">
-        <v>456</v>
+        <v>492</v>
       </c>
       <c r="C15" s="92"/>
       <c r="D15" s="69"/>
@@ -53188,10 +53728,10 @@
     </row>
     <row r="16" ht="16" customHeight="1">
       <c r="A16" t="s" s="80">
-        <v>467</v>
+        <v>503</v>
       </c>
       <c r="B16" t="s" s="81">
-        <v>468</v>
+        <v>504</v>
       </c>
       <c r="C16" s="82"/>
       <c r="D16" s="69"/>
@@ -53228,7 +53768,7 @@
     </row>
     <row r="18" ht="19" customHeight="1">
       <c r="A18" t="s" s="43">
-        <v>469</v>
+        <v>505</v>
       </c>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -53249,7 +53789,7 @@
     <row r="19" ht="19" customHeight="1">
       <c r="A19" s="79"/>
       <c r="B19" t="s" s="77">
-        <v>450</v>
+        <v>486</v>
       </c>
       <c r="C19" t="s" s="78">
         <v>2</v>
@@ -53270,10 +53810,10 @@
     </row>
     <row r="20" ht="16" customHeight="1">
       <c r="A20" t="s" s="80">
-        <v>470</v>
+        <v>506</v>
       </c>
       <c r="B20" t="s" s="81">
-        <v>471</v>
+        <v>507</v>
       </c>
       <c r="C20" s="82"/>
       <c r="D20" s="69"/>
@@ -53293,7 +53833,7 @@
     <row r="21" ht="16" customHeight="1">
       <c r="A21" s="84"/>
       <c r="B21" t="s" s="85">
-        <v>460</v>
+        <v>496</v>
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="69"/>
@@ -53312,13 +53852,13 @@
     </row>
     <row r="22" ht="16" customHeight="1">
       <c r="A22" t="s" s="81">
-        <v>472</v>
+        <v>508</v>
       </c>
       <c r="B22" t="s" s="81">
-        <v>473</v>
+        <v>509</v>
       </c>
       <c r="C22" t="s" s="80">
-        <v>474</v>
+        <v>510</v>
       </c>
       <c r="D22" s="69"/>
       <c r="E22" s="69"/>
@@ -53335,13 +53875,13 @@
     </row>
     <row r="23" ht="16" customHeight="1">
       <c r="A23" t="s" s="81">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B23" t="s" s="81">
-        <v>476</v>
+        <v>512</v>
       </c>
       <c r="C23" t="s" s="80">
-        <v>477</v>
+        <v>513</v>
       </c>
       <c r="D23" s="69"/>
       <c r="E23" s="69"/>
@@ -53359,7 +53899,7 @@
     <row r="24" ht="16" customHeight="1">
       <c r="A24" s="92"/>
       <c r="B24" t="s" s="85">
-        <v>456</v>
+        <v>492</v>
       </c>
       <c r="C24" t="s" s="93">
         <v>2</v>
@@ -53379,10 +53919,10 @@
     </row>
     <row r="25" ht="16" customHeight="1">
       <c r="A25" t="s" s="33">
-        <v>478</v>
+        <v>514</v>
       </c>
       <c r="B25" t="s" s="81">
-        <v>479</v>
+        <v>515</v>
       </c>
       <c r="C25" s="82"/>
       <c r="D25" s="69"/>
@@ -53400,10 +53940,10 @@
     </row>
     <row r="26" ht="16" customHeight="1">
       <c r="A26" t="s" s="33">
-        <v>480</v>
+        <v>516</v>
       </c>
       <c r="B26" t="s" s="81">
-        <v>481</v>
+        <v>517</v>
       </c>
       <c r="C26" s="82"/>
       <c r="D26" s="69"/>
@@ -53422,7 +53962,7 @@
     <row r="27" ht="16" customHeight="1">
       <c r="A27" s="94"/>
       <c r="B27" t="s" s="85">
-        <v>482</v>
+        <v>518</v>
       </c>
       <c r="C27" s="94"/>
       <c r="D27" s="69"/>
@@ -53440,10 +53980,10 @@
     </row>
     <row r="28" ht="16" customHeight="1">
       <c r="A28" t="s" s="33">
-        <v>483</v>
+        <v>519</v>
       </c>
       <c r="B28" t="s" s="81">
-        <v>484</v>
+        <v>520</v>
       </c>
       <c r="C28" s="82"/>
       <c r="D28" s="69"/>
@@ -53478,7 +54018,7 @@
     </row>
     <row r="30" ht="19" customHeight="1">
       <c r="A30" t="s" s="43">
-        <v>449</v>
+        <v>485</v>
       </c>
       <c r="B30" s="44"/>
       <c r="C30" s="71"/>
@@ -53498,7 +54038,7 @@
     <row r="31" ht="16" customHeight="1">
       <c r="A31" s="95"/>
       <c r="B31" t="s" s="78">
-        <v>460</v>
+        <v>496</v>
       </c>
       <c r="C31" t="s" s="96">
         <v>2</v>
@@ -53509,13 +54049,13 @@
         <v>1</v>
       </c>
       <c r="G31" t="s" s="85">
-        <v>485</v>
+        <v>521</v>
       </c>
       <c r="H31" t="s" s="85">
-        <v>486</v>
+        <v>522</v>
       </c>
       <c r="I31" t="s" s="85">
-        <v>487</v>
+        <v>523</v>
       </c>
       <c r="J31" s="69"/>
       <c r="K31" s="69"/>
@@ -53526,10 +54066,10 @@
     </row>
     <row r="32" ht="16" customHeight="1">
       <c r="A32" t="s" s="81">
-        <v>488</v>
+        <v>524</v>
       </c>
       <c r="B32" t="s" s="81">
-        <v>390</v>
+        <v>426</v>
       </c>
       <c r="C32" s="82"/>
       <c r="D32" s="69"/>
@@ -53547,10 +54087,10 @@
     </row>
     <row r="33" ht="16" customHeight="1">
       <c r="A33" t="s" s="81">
-        <v>489</v>
+        <v>525</v>
       </c>
       <c r="B33" t="s" s="81">
-        <v>490</v>
+        <v>526</v>
       </c>
       <c r="C33" s="82"/>
       <c r="D33" s="69"/>
@@ -53568,10 +54108,10 @@
     </row>
     <row r="34" ht="16" customHeight="1">
       <c r="A34" t="s" s="81">
-        <v>491</v>
+        <v>527</v>
       </c>
       <c r="B34" t="s" s="81">
-        <v>492</v>
+        <v>528</v>
       </c>
       <c r="C34" s="82"/>
       <c r="D34" s="69"/>
@@ -53589,13 +54129,13 @@
     </row>
     <row r="35" ht="16" customHeight="1">
       <c r="A35" t="s" s="81">
-        <v>493</v>
+        <v>529</v>
       </c>
       <c r="B35" t="s" s="81">
-        <v>494</v>
+        <v>530</v>
       </c>
       <c r="C35" t="s" s="80">
-        <v>495</v>
+        <v>531</v>
       </c>
       <c r="D35" s="69"/>
       <c r="E35" s="69"/>
@@ -53612,10 +54152,10 @@
     </row>
     <row r="36" ht="16" customHeight="1">
       <c r="A36" t="s" s="81">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="B36" t="s" s="81">
-        <v>497</v>
+        <v>533</v>
       </c>
       <c r="C36" s="82"/>
       <c r="D36" s="69"/>
@@ -53633,10 +54173,10 @@
     </row>
     <row r="37" ht="16" customHeight="1">
       <c r="A37" t="s" s="81">
-        <v>498</v>
+        <v>534</v>
       </c>
       <c r="B37" t="s" s="81">
-        <v>499</v>
+        <v>535</v>
       </c>
       <c r="C37" s="82"/>
       <c r="D37" s="69"/>
@@ -53654,10 +54194,10 @@
     </row>
     <row r="38" ht="16" customHeight="1">
       <c r="A38" t="s" s="81">
-        <v>500</v>
+        <v>536</v>
       </c>
       <c r="B38" t="s" s="81">
-        <v>501</v>
+        <v>537</v>
       </c>
       <c r="C38" s="82"/>
       <c r="D38" s="69"/>
@@ -53676,7 +54216,7 @@
     <row r="39" ht="16" customHeight="1">
       <c r="A39" s="94"/>
       <c r="B39" t="s" s="85">
-        <v>456</v>
+        <v>492</v>
       </c>
       <c r="C39" s="94"/>
       <c r="D39" s="69"/>
@@ -53684,16 +54224,16 @@
       <c r="F39" s="69"/>
       <c r="G39" s="69"/>
       <c r="H39" t="s" s="98">
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="I39" t="s" s="98">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="J39" t="s" s="98">
-        <v>504</v>
+        <v>540</v>
       </c>
       <c r="K39" t="s" s="98">
-        <v>505</v>
+        <v>541</v>
       </c>
       <c r="L39" s="69"/>
       <c r="M39" s="83">
@@ -53702,10 +54242,10 @@
     </row>
     <row r="40" ht="18" customHeight="1">
       <c r="A40" t="s" s="80">
-        <v>506</v>
+        <v>542</v>
       </c>
       <c r="B40" t="s" s="81">
-        <v>507</v>
+        <v>543</v>
       </c>
       <c r="C40" s="82"/>
       <c r="D40" s="69"/>
@@ -53723,10 +54263,10 @@
     </row>
     <row r="41" ht="18" customHeight="1">
       <c r="A41" t="s" s="80">
-        <v>508</v>
+        <v>544</v>
       </c>
       <c r="B41" t="s" s="81">
-        <v>509</v>
+        <v>545</v>
       </c>
       <c r="C41" s="82"/>
       <c r="D41" s="69"/>
@@ -53745,7 +54285,7 @@
     <row r="42" ht="18" customHeight="1">
       <c r="A42" s="94"/>
       <c r="B42" t="s" s="85">
-        <v>510</v>
+        <v>546</v>
       </c>
       <c r="C42" s="94"/>
       <c r="D42" s="69"/>
@@ -53754,10 +54294,10 @@
       <c r="G42" s="69"/>
       <c r="H42" s="99"/>
       <c r="I42" t="s" s="85">
-        <v>511</v>
+        <v>547</v>
       </c>
       <c r="J42" t="s" s="85">
-        <v>512</v>
+        <v>548</v>
       </c>
       <c r="K42" s="69"/>
       <c r="L42" s="69"/>
@@ -53767,10 +54307,10 @@
     </row>
     <row r="43" ht="16" customHeight="1">
       <c r="A43" t="s" s="33">
-        <v>513</v>
+        <v>549</v>
       </c>
       <c r="B43" t="s" s="81">
-        <v>514</v>
+        <v>550</v>
       </c>
       <c r="C43" s="82"/>
       <c r="D43" s="69"/>
@@ -53788,13 +54328,13 @@
     </row>
     <row r="44" ht="16" customHeight="1">
       <c r="A44" t="s" s="80">
-        <v>515</v>
+        <v>551</v>
       </c>
       <c r="B44" t="s" s="80">
-        <v>516</v>
+        <v>552</v>
       </c>
       <c r="C44" t="s" s="80">
-        <v>517</v>
+        <v>553</v>
       </c>
       <c r="D44" s="69"/>
       <c r="E44" s="69"/>
@@ -53811,10 +54351,10 @@
     </row>
     <row r="45" ht="16" customHeight="1">
       <c r="A45" t="s" s="80">
-        <v>518</v>
+        <v>554</v>
       </c>
       <c r="B45" t="s" s="81">
-        <v>519</v>
+        <v>555</v>
       </c>
       <c r="C45" s="82"/>
       <c r="D45" s="69"/>
@@ -53832,10 +54372,10 @@
     </row>
     <row r="46" ht="16" customHeight="1">
       <c r="A46" t="s" s="80">
-        <v>520</v>
+        <v>556</v>
       </c>
       <c r="B46" t="s" s="81">
-        <v>521</v>
+        <v>557</v>
       </c>
       <c r="C46" s="82"/>
       <c r="D46" s="69"/>
@@ -53853,10 +54393,10 @@
     </row>
     <row r="47" ht="16" customHeight="1">
       <c r="A47" t="s" s="80">
-        <v>522</v>
+        <v>558</v>
       </c>
       <c r="B47" t="s" s="81">
-        <v>523</v>
+        <v>559</v>
       </c>
       <c r="C47" s="82"/>
       <c r="D47" s="69"/>
@@ -53874,13 +54414,13 @@
     </row>
     <row r="48" ht="16" customHeight="1">
       <c r="A48" t="s" s="80">
-        <v>524</v>
+        <v>560</v>
       </c>
       <c r="B48" t="s" s="81">
-        <v>525</v>
+        <v>561</v>
       </c>
       <c r="C48" t="s" s="80">
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="D48" s="69"/>
       <c r="E48" s="69"/>
@@ -53897,13 +54437,13 @@
     </row>
     <row r="49" ht="16" customHeight="1">
       <c r="A49" t="s" s="80">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="B49" t="s" s="81">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="C49" t="s" s="80">
-        <v>529</v>
+        <v>565</v>
       </c>
       <c r="D49" s="69"/>
       <c r="E49" s="69"/>
@@ -53920,13 +54460,13 @@
     </row>
     <row r="50" ht="16" customHeight="1">
       <c r="A50" t="s" s="80">
-        <v>530</v>
+        <v>566</v>
       </c>
       <c r="B50" t="s" s="81">
-        <v>531</v>
+        <v>567</v>
       </c>
       <c r="C50" t="s" s="80">
-        <v>532</v>
+        <v>568</v>
       </c>
       <c r="D50" s="69"/>
       <c r="E50" s="69"/>
@@ -53943,13 +54483,13 @@
     </row>
     <row r="51" ht="16" customHeight="1">
       <c r="A51" t="s" s="80">
-        <v>533</v>
+        <v>569</v>
       </c>
       <c r="B51" t="s" s="81">
-        <v>534</v>
+        <v>570</v>
       </c>
       <c r="C51" t="s" s="80">
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="D51" s="69"/>
       <c r="E51" s="69"/>
@@ -53966,13 +54506,13 @@
     </row>
     <row r="52" ht="16" customHeight="1">
       <c r="A52" t="s" s="80">
-        <v>535</v>
+        <v>571</v>
       </c>
       <c r="B52" t="s" s="81">
-        <v>536</v>
+        <v>572</v>
       </c>
       <c r="C52" t="s" s="80">
-        <v>529</v>
+        <v>565</v>
       </c>
       <c r="D52" s="69"/>
       <c r="E52" s="69"/>
@@ -53990,22 +54530,22 @@
     <row r="53" ht="16" customHeight="1">
       <c r="A53" s="94"/>
       <c r="B53" t="s" s="85">
-        <v>537</v>
+        <v>573</v>
       </c>
       <c r="C53" s="94"/>
       <c r="D53" s="69"/>
       <c r="E53" s="69"/>
       <c r="F53" t="s" s="85">
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="G53" t="s" s="85">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="H53" t="s" s="85">
-        <v>504</v>
+        <v>540</v>
       </c>
       <c r="I53" t="s" s="85">
-        <v>505</v>
+        <v>541</v>
       </c>
       <c r="J53" s="69"/>
       <c r="K53" s="69"/>
@@ -54016,10 +54556,10 @@
     </row>
     <row r="54" ht="16" customHeight="1">
       <c r="A54" t="s" s="81">
-        <v>538</v>
+        <v>574</v>
       </c>
       <c r="B54" t="s" s="81">
-        <v>539</v>
+        <v>575</v>
       </c>
       <c r="C54" s="82"/>
       <c r="D54" s="69"/>
@@ -54037,10 +54577,10 @@
     </row>
     <row r="55" ht="16" customHeight="1">
       <c r="A55" t="s" s="81">
-        <v>540</v>
+        <v>576</v>
       </c>
       <c r="B55" t="s" s="81">
-        <v>541</v>
+        <v>577</v>
       </c>
       <c r="C55" s="82"/>
       <c r="D55" s="69"/>
@@ -54058,10 +54598,10 @@
     </row>
     <row r="56" ht="16" customHeight="1">
       <c r="A56" t="s" s="81">
-        <v>542</v>
+        <v>578</v>
       </c>
       <c r="B56" t="s" s="81">
-        <v>543</v>
+        <v>579</v>
       </c>
       <c r="C56" s="82"/>
       <c r="D56" s="69"/>
@@ -54079,10 +54619,10 @@
     </row>
     <row r="57" ht="16" customHeight="1">
       <c r="A57" t="s" s="81">
-        <v>544</v>
+        <v>580</v>
       </c>
       <c r="B57" t="s" s="81">
-        <v>545</v>
+        <v>581</v>
       </c>
       <c r="C57" s="69"/>
       <c r="D57" s="69"/>
@@ -54117,10 +54657,10 @@
     </row>
     <row r="59" ht="16" customHeight="1">
       <c r="A59" t="s" s="81">
-        <v>546</v>
+        <v>582</v>
       </c>
       <c r="B59" t="s" s="81">
-        <v>547</v>
+        <v>583</v>
       </c>
       <c r="C59" s="69"/>
       <c r="D59" s="69"/>
@@ -54138,10 +54678,10 @@
     </row>
     <row r="60" ht="16" customHeight="1">
       <c r="A60" t="s" s="81">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="B60" t="s" s="81">
-        <v>549</v>
+        <v>585</v>
       </c>
       <c r="C60" s="69"/>
       <c r="D60" s="69"/>

</xml_diff>